<commit_message>
fix return data timeout
json stringsify page.evaliuate return data to reduce data complexity and size
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -489,7 +489,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I2" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J2" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -514,7 +514,7 @@
         <v>1พัน</v>
       </c>
       <c r="M2" t="str">
-        <v>539</v>
+        <v>522</v>
       </c>
       <c r="N2" t="str">
         <v>฿25</v>
@@ -525,7 +525,7 @@
       <c r="P2" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -565,7 +565,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I3" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J3" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -590,7 +590,7 @@
         <v>1พัน</v>
       </c>
       <c r="M3" t="str">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="N3" t="str">
         <v>฿45</v>
@@ -601,7 +601,7 @@
       <c r="P3" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -641,7 +641,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I4" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J4" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -666,7 +666,7 @@
         <v>1พัน</v>
       </c>
       <c r="M4" t="str">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="N4" t="str">
         <v>฿55</v>
@@ -677,7 +677,7 @@
       <c r="P4" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -717,7 +717,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I5" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J5" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -753,7 +753,7 @@
       <c r="P5" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -793,7 +793,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I6" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J6" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -818,7 +818,7 @@
         <v>1พัน</v>
       </c>
       <c r="M6" t="str">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="N6" t="str">
         <v>฿25</v>
@@ -829,7 +829,7 @@
       <c r="P6" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -869,7 +869,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I7" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J7" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -894,7 +894,7 @@
         <v>1พัน</v>
       </c>
       <c r="M7" t="str">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="N7" t="str">
         <v>฿45</v>
@@ -905,7 +905,7 @@
       <c r="P7" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -945,7 +945,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I8" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J8" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -970,7 +970,7 @@
         <v>1พัน</v>
       </c>
       <c r="M8" t="str">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="N8" t="str">
         <v>฿55</v>
@@ -981,7 +981,7 @@
       <c r="P8" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I9" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J9" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -1057,7 +1057,7 @@
       <c r="P9" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I10" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J10" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -1122,7 +1122,7 @@
         <v>1พัน</v>
       </c>
       <c r="M10" t="str">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="N10" t="str">
         <v>฿25</v>
@@ -1133,7 +1133,7 @@
       <c r="P10" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I11" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J11" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -1198,7 +1198,7 @@
         <v>1พัน</v>
       </c>
       <c r="M11" t="str">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N11" t="str">
         <v>฿45</v>
@@ -1209,7 +1209,7 @@
       <c r="P11" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I12" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J12" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -1285,7 +1285,7 @@
       <c r="P12" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>฿16 - ฿55</v>
       </c>
       <c r="I13" t="str">
-        <v>3821</v>
+        <v>3749</v>
       </c>
       <c r="J13" t="str" xml:space="preserve">
         <v xml:space="preserve">มีดตัดขนมปังสแตนเลสแท้ MAXIE (มีให้เลือกถึง 3 แบบ = แบบเรียบ, แบบซี่ถี่, แบบซี่ห่าง :3 ขนาด= 10, 12, 14 นิ้ว) พร้อมกับด้ามจับแบบไม้พิเศษ โดยมีดแต่ละประเภทจะมีการใช้งานที่แตกต่างกันออกไป ดังนี้ 
@@ -1350,7 +1350,7 @@
         <v>1พัน</v>
       </c>
       <c r="M13" t="str">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="N13" t="str">
         <v>฿16</v>
@@ -1361,7 +1361,7 @@
       <c r="P13" t="str" xml:space="preserve">
         <v xml:space="preserve">{
   "หมวดหมู่": "Shopee&gt;เครื่องใช้ในบ้าน&gt;ห้องครัวและห้องอาหาร&gt;อุปกรณ์เบ็ดเตล็ดในครัวอื่นๆ",
-  "จำนวนสินค้า": "3821",
+  "จำนวนสินค้า": "3749",
   "ส่งจาก": "จังหวัดราชบุรี"
 }</v>
       </c>
@@ -1426,10 +1426,10 @@
         <v>wanna__shop</v>
       </c>
       <c r="C2" t="str">
-        <v>177.5พัน</v>
+        <v>178พัน</v>
       </c>
       <c r="D2" t="str">
-        <v>98%</v>
+        <v>97%</v>
       </c>
       <c r="E2" t="str">
         <v>3 ปี ที่ผ่านมา</v>
@@ -1438,7 +1438,7 @@
         <v>ภายในไม่กี่ชั่วโมง</v>
       </c>
       <c r="G2" t="str">
-        <v>99.9พัน</v>
+        <v>100.1พัน</v>
       </c>
       <c r="H2" t="str">
         <v>https://shopee.co.th/wanna__shop?categoryId=100636&amp;entryPoint=ShopByPDP&amp;itemId=4960495896</v>

</xml_diff>